<commit_message>
tweaking things in unity and writing more as we reach the true true end
</commit_message>
<xml_diff>
--- a/auto-animation/testing/PathEstimateValueChecking.xlsx
+++ b/auto-animation/testing/PathEstimateValueChecking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>v0</t>
   </si>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection sqref="A1:AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,12 +4178,1530 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>(G2-D2)/M2 - (J2 * M2)/2</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <f>(H2-E2)/M2 - (K2 * M2)/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="1">
+        <f>(I2-F2)/M2 - (L2 * M2)/2</f>
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>-10</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N2">
+        <f>A2/Q2</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>B2/Q2</f>
+        <v>2.5</v>
+      </c>
+      <c r="P2">
+        <f>C2/Q2</f>
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R2">
+        <f>SQRT(A2^2 + B2^2 + C2^2)</f>
+        <v>10.012492197250394</v>
+      </c>
+      <c r="S2" s="1">
+        <f>SQRT(N2^2+O2^2 +P2^2)</f>
+        <v>50.062460986251963</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="V2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W2" s="1">
+        <f>1/2 * V2 * U2^2</f>
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0.01</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z2" s="2">
+        <f>1/2 * Y2 * X2^2</f>
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC2" s="1">
+        <f>1/2 * AB2 * AA2^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A16" si="0">(G3-D3)/M3 - (J3 * M3)/2</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B16" si="1">(H3-E3)/M3 - (K3 * M3)/2</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C16" si="2">(I3-F3)/M3 - (L3 * M3)/2</f>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>-10</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N16" si="3">A3/Q3</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O16" si="4">B3/Q3</f>
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P16" si="5">C3/Q3</f>
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R16" si="6">SQRT(A3^2 + B3^2 + C3^2)</f>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="S3" s="1">
+        <f t="shared" ref="S3:S16" si="7">SQRT(N3^2+O3^2 +P3^2)</f>
+        <v>25.495097567963924</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="V3" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W3" s="1">
+        <f t="shared" ref="W3:W16" si="8">1/2 * V3 * U3^2</f>
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>0.02</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z3" s="2">
+        <f t="shared" ref="Z3:Z16" si="9">1/2 * Y3 * X3^2</f>
+        <v>4</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC3" s="1">
+        <f t="shared" ref="AC3:AC16" si="10">1/2 * AB3 * AA3^2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>-10</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>7.5</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="5"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="6"/>
+        <v>3.655285366576885</v>
+      </c>
+      <c r="S4" s="1">
+        <f t="shared" si="7"/>
+        <v>18.276426832884425</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="V4" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="X4">
+        <v>0.03</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC4" s="1">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>-10</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="6"/>
+        <v>3.2015621187164243</v>
+      </c>
+      <c r="S5" s="1">
+        <f t="shared" si="7"/>
+        <v>16.007810593582121</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="V5" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="X5">
+        <v>0.04</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z5" s="2">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>-10</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="6"/>
+        <v>3.2015621187164243</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="7"/>
+        <v>16.007810593582121</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="V6" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="8"/>
+        <v>25.000000000000004</v>
+      </c>
+      <c r="X6">
+        <v>0.05</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z6" s="2">
+        <f t="shared" si="9"/>
+        <v>25.000000000000004</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC6" s="1">
+        <f t="shared" si="10"/>
+        <v>25.000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>-10</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="6"/>
+        <v>3.4318767136623336</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" si="7"/>
+        <v>17.159383568311668</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="V7" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="X7">
+        <v>0.06</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z7" s="2">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC7" s="1">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>-10</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>17.5</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="6"/>
+        <v>3.7803196063997833</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" si="7"/>
+        <v>18.901598031998915</v>
+      </c>
+      <c r="U8" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="8"/>
+        <v>49.000000000000007</v>
+      </c>
+      <c r="X8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="9"/>
+        <v>49.000000000000007</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" si="10"/>
+        <v>49.000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>-10</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="5"/>
+        <v>6.25</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="6"/>
+        <v>4.1907636535600528</v>
+      </c>
+      <c r="S9" s="1">
+        <f t="shared" si="7"/>
+        <v>20.953818267800262</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="V9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="X9">
+        <v>0.08</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z9" s="2">
+        <f t="shared" si="9"/>
+        <v>64</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC9" s="1">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>-10</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>22.5</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="6"/>
+        <v>4.6351448630258112</v>
+      </c>
+      <c r="S10" s="1">
+        <f t="shared" si="7"/>
+        <v>23.175724315129056</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="V10" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="8"/>
+        <v>81</v>
+      </c>
+      <c r="X10">
+        <v>0.09</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z10" s="2">
+        <f t="shared" si="9"/>
+        <v>81</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC10" s="1">
+        <f t="shared" si="10"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>-10</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="6"/>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="S11" s="1">
+        <f t="shared" si="7"/>
+        <v>25.495097567963924</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" si="8"/>
+        <v>100.00000000000001</v>
+      </c>
+      <c r="X11">
+        <v>0.1</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z11" s="2">
+        <f t="shared" si="9"/>
+        <v>100.00000000000001</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="10"/>
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>-10</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>27.5</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>4.545454545454545</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="6"/>
+        <v>5.5746252143970842</v>
+      </c>
+      <c r="S12" s="1">
+        <f t="shared" si="7"/>
+        <v>27.873126071985421</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="V12" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W12" s="1">
+        <f t="shared" si="8"/>
+        <v>121</v>
+      </c>
+      <c r="X12">
+        <v>0.11</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z12" s="2">
+        <f t="shared" si="9"/>
+        <v>121</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="10"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>-10</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="6"/>
+        <v>6.0575939484620829</v>
+      </c>
+      <c r="S13" s="1">
+        <f t="shared" si="7"/>
+        <v>30.287969742310413</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="V13" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W13" s="1">
+        <f t="shared" si="8"/>
+        <v>144</v>
+      </c>
+      <c r="X13">
+        <v>0.12</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z13" s="2">
+        <f t="shared" si="9"/>
+        <v>144</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="10"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.76923076923076916</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>-10</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>32.5</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>3.8461538461538458</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="6"/>
+        <v>6.5453583535457671</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" si="7"/>
+        <v>32.726791767728841</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="V14" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W14" s="1">
+        <f t="shared" si="8"/>
+        <v>169.00000000000003</v>
+      </c>
+      <c r="X14">
+        <v>0.13</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z14" s="2">
+        <f t="shared" si="9"/>
+        <v>169.00000000000003</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC14" s="1">
+        <f t="shared" si="10"/>
+        <v>169.00000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>-10</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="5"/>
+        <v>3.5714285714285712</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="6"/>
+        <v>7.0363487748712865</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="7"/>
+        <v>35.181743874356435</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V15" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W15" s="1">
+        <f t="shared" si="8"/>
+        <v>196.00000000000003</v>
+      </c>
+      <c r="X15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z15" s="2">
+        <f t="shared" si="9"/>
+        <v>196.00000000000003</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC15" s="1">
+        <f t="shared" si="10"/>
+        <v>196.00000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>-10</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>37.5</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="5"/>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="6"/>
+        <v>7.5295713320510114</v>
+      </c>
+      <c r="S16" s="1">
+        <f t="shared" si="7"/>
+        <v>37.647856660255059</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="V16" s="1">
+        <v>20000</v>
+      </c>
+      <c r="W16" s="1">
+        <f t="shared" si="8"/>
+        <v>225</v>
+      </c>
+      <c r="X16">
+        <v>0.15</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>20000</v>
+      </c>
+      <c r="Z16" s="2">
+        <f t="shared" si="9"/>
+        <v>225</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>20000</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" si="10"/>
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>